<commit_message>
Initial Creation of Delivery History and Updated Project Plan and RTM Signed-off-by: moamen-ahmed-93 <moamen.ahmed.9930@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\Input documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A013E-0F78-4700-B192-BF704E343A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction " sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Cross review points " sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Introduction " sheetId="1" r:id="rId1"/>
+    <sheet name="Cross review points " sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_Toc30697436" vbProcedure="false">#REF!</definedName>
+    <definedName name="_Toc30697436" localSheetId="1">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -41,28 +46,28 @@
     <t xml:space="preserve">Ref Version </t>
   </si>
   <si>
-    <t xml:space="preserve">Initial Version</t>
+    <t>Initial Version</t>
   </si>
   <si>
     <t xml:space="preserve">Author </t>
   </si>
   <si>
-    <t xml:space="preserve">Abdelrahman Ali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31/01/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
+    <t>Abdelrahman Ali</t>
+  </si>
+  <si>
+    <t>Last update</t>
+  </si>
+  <si>
+    <t>31/01/2020</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Author</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -71,93 +76,93 @@
     <t xml:space="preserve">Change </t>
   </si>
   <si>
-    <t xml:space="preserve">A.Ali</t>
+    <t>A.Ali</t>
   </si>
   <si>
     <t xml:space="preserve">Initial creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Entry Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Detection version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page/Line/Section/Entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open point : description of problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
+    <t>Entry Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Detection version</t>
+  </si>
+  <si>
+    <t>Name of file</t>
+  </si>
+  <si>
+    <t>Page/Line/Section/Entity</t>
+  </si>
+  <si>
+    <t>Open point : description of problem</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
   <si>
     <t xml:space="preserve">Initial Version </t>
   </si>
   <si>
-    <t xml:space="preserve">CYRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page 1</t>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>Page 1</t>
   </si>
   <si>
     <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Releases after accomplishing cross review on it. </t>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The version of CYRS document isn’t defined and some pages left blank without any data.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last page</t>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>All pages</t>
+  </si>
+  <si>
+    <t>The version of CYRS document isn’t defined and some pages left blank without any data.</t>
+  </si>
+  <si>
+    <t>Last page</t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even CYRS should have one and the reference is the customer Requirement for the product </t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document History</t>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Document History</t>
   </si>
   <si>
     <t xml:space="preserve">Document history has to be at the start &amp; status of document should be draft and after the cross review is done and 
 points fixed then it could be proposed </t>
   </si>
   <si>
-    <t xml:space="preserve">Refused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of Figures</t>
+    <t>Refused</t>
+  </si>
+  <si>
+    <t>List of Figures</t>
   </si>
   <si>
     <t xml:space="preserve">List of figures page is blank if you didn’t plan to put data on it you should delete it. </t>
   </si>
   <si>
-    <t xml:space="preserve">Page 6 &amp; Page 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There’s no need to write chapter number (Chapter 1 , 2 , 3) above the section because the scope of CYRS document to explain 
+    <t>Page 6 &amp; Page 7</t>
+  </si>
+  <si>
+    <t>There’s no need to write chapter number (Chapter 1 , 2 , 3) above the section because the scope of CYRS document to explain 
 The system requirements and it isn’t like a book or a novel.</t>
   </si>
   <si>
-    <t xml:space="preserve">Page 7</t>
+    <t>Page 7</t>
   </si>
   <si>
     <t xml:space="preserve">There is no need to define a section for Hardware components in CYRS and instead of that you need to describe 
@@ -167,7 +172,7 @@
     <t xml:space="preserve">Page 8 </t>
   </si>
   <si>
-    <t xml:space="preserve">Project History header should be deleted and the points in Software Section should be defined as requirements
+    <t>Project History header should be deleted and the points in Software Section should be defined as requirements
  with a separate requirement ID for each point.</t>
   </si>
   <si>
@@ -181,10 +186,10 @@
 operation button”. </t>
   </si>
   <si>
-    <t xml:space="preserve">Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Should define an appropriate title for the table you used to put a content or data on it to be expressed 
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Should define an appropriate title for the table you used to put a content or data on it to be expressed 
 So, need to change the title of the table defined in Features section.</t>
   </si>
   <si>
@@ -217,7 +222,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Req PO1 DGC CYRS 001 v1.0</t>
+      <t>Req PO1 DGC CYRS 001 v1.0</t>
     </r>
     <r>
       <rPr>
@@ -250,7 +255,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Resolved</t>
+    <t>Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Decision </t>
@@ -268,17 +273,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="168" formatCode="[$-409]General"/>
-    <numFmt numFmtId="169" formatCode="[$-409]M/D/YYYY"/>
-    <numFmt numFmtId="170" formatCode="@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]General"/>
+    <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -287,22 +289,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -310,7 +297,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -333,6 +320,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -366,103 +360,149 @@
     </fill>
   </fills>
   <borders count="11">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
       <top style="medium">
         <color rgb="FF70AD47"/>
       </top>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF70AD47"/>
       </left>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF70AD47"/>
       </right>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color rgb="FF70AD47"/>
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -478,219 +518,159 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Normal 3 2" xfId="20"/>
-    <cellStyle name="Normal 4" xfId="21"/>
-    <cellStyle name="Excel Built-in Accent3" xfId="22"/>
+    <cellStyle name="Normal 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF808080"/>
+        <color rgb="FFFBE5D6"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF535353"/>
       </font>
@@ -702,41 +682,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF385724"/>
+        <color rgb="FF808080"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -795,224 +752,535 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF385724"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:M18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:M18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11" t="n">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="14">
         <v>0.1</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="3"/>
+      <c r="G13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
@@ -1020,56 +1288,45 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="106.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="174.28"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="106.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:11" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
@@ -1098,7 +1355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
@@ -1117,13 +1374,15 @@
       <c r="F2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H2" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -1142,13 +1401,15 @@
       <c r="F3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H3" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
@@ -1167,16 +1428,18 @@
       <c r="F4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H4" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="24"/>
-      <c r="K4" s="0" t="s">
+      <c r="K4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>9</v>
       </c>
@@ -1195,16 +1458,18 @@
       <c r="F5" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H5" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="24"/>
-      <c r="K5" s="0" t="s">
+      <c r="K5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
@@ -1223,13 +1488,15 @@
       <c r="F6" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H6" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="24"/>
     </row>
-    <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
@@ -1248,13 +1515,15 @@
       <c r="F7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H7" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
@@ -1273,13 +1542,15 @@
       <c r="F8" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H8" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
@@ -1298,13 +1569,15 @@
       <c r="F9" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H9" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>9</v>
       </c>
@@ -1323,13 +1596,15 @@
       <c r="F10" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H10" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>9</v>
       </c>
@@ -1348,13 +1623,15 @@
       <c r="F11" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" customFormat="false" ht="37.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1373,13 +1650,15 @@
       <c r="F12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>9</v>
       </c>
@@ -1398,13 +1677,15 @@
       <c r="F13" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
@@ -1416,11 +1697,11 @@
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
       <c r="I14" s="22"/>
-      <c r="K14" s="0" t="s">
+      <c r="K14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
@@ -1431,7 +1712,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
@@ -1442,7 +1723,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="22"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
@@ -1452,14 +1733,14 @@
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="22"/>
-      <c r="K17" s="0" t="s">
+      <c r="K17" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="0" t="s">
+      <c r="L17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
@@ -1469,14 +1750,14 @@
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
       <c r="I18" s="22"/>
-      <c r="K18" s="0" t="s">
+      <c r="K18" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="0" t="s">
+      <c r="L18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -1487,7 +1768,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21"/>
@@ -1498,7 +1779,7 @@
       <c r="H20" s="24"/>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
@@ -1509,7 +1790,7 @@
       <c r="H21" s="24"/>
       <c r="I21" s="22"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -1520,7 +1801,7 @@
       <c r="H22" s="24"/>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -1531,7 +1812,7 @@
       <c r="H23" s="24"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="30"/>
@@ -1542,7 +1823,7 @@
       <c r="H24" s="24"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="30"/>
@@ -1553,7 +1834,7 @@
       <c r="H25" s="24"/>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="29"/>
       <c r="C26" s="30"/>
@@ -1564,7 +1845,7 @@
       <c r="H26" s="24"/>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="29"/>
       <c r="C27" s="30"/>
@@ -1575,7 +1856,7 @@
       <c r="H27" s="24"/>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="29"/>
       <c r="C28" s="30"/>
@@ -1586,7 +1867,7 @@
       <c r="H28" s="24"/>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="29"/>
       <c r="C29" s="30"/>
@@ -1597,7 +1878,7 @@
       <c r="H29" s="24"/>
       <c r="I29" s="33"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="29"/>
       <c r="C30" s="30"/>
@@ -1608,7 +1889,7 @@
       <c r="H30" s="24"/>
       <c r="I30" s="33"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="29"/>
       <c r="C31" s="30"/>
@@ -1619,7 +1900,7 @@
       <c r="H31" s="24"/>
       <c r="I31" s="33"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
       <c r="B32" s="29"/>
       <c r="C32" s="30"/>
@@ -1630,7 +1911,7 @@
       <c r="H32" s="24"/>
       <c r="I32" s="33"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="29"/>
       <c r="C33" s="30"/>
@@ -1641,7 +1922,7 @@
       <c r="H33" s="24"/>
       <c r="I33" s="33"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -1652,7 +1933,7 @@
       <c r="H34" s="24"/>
       <c r="I34" s="33"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
@@ -1663,7 +1944,7 @@
       <c r="H35" s="24"/>
       <c r="I35" s="33"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
@@ -1674,7 +1955,7 @@
       <c r="H36" s="24"/>
       <c r="I36" s="33"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -1685,7 +1966,7 @@
       <c r="H37" s="24"/>
       <c r="I37" s="33"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -1696,7 +1977,7 @@
       <c r="H38" s="24"/>
       <c r="I38" s="33"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -1707,7 +1988,7 @@
       <c r="H39" s="24"/>
       <c r="I39" s="33"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -1718,7 +1999,7 @@
       <c r="H40" s="24"/>
       <c r="I40" s="33"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -1729,7 +2010,7 @@
       <c r="H41" s="24"/>
       <c r="I41" s="33"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -1740,7 +2021,7 @@
       <c r="H42" s="24"/>
       <c r="I42" s="33"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="30"/>
       <c r="C43" s="30"/>
@@ -1751,7 +2032,7 @@
       <c r="H43" s="24"/>
       <c r="I43" s="33"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="30"/>
       <c r="C44" s="30"/>
@@ -1762,7 +2043,7 @@
       <c r="H44" s="24"/>
       <c r="I44" s="33"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="30"/>
       <c r="C45" s="30"/>
@@ -1773,7 +2054,7 @@
       <c r="H45" s="24"/>
       <c r="I45" s="33"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="30"/>
       <c r="C46" s="30"/>
@@ -1784,7 +2065,7 @@
       <c r="H46" s="24"/>
       <c r="I46" s="33"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="30"/>
       <c r="C47" s="30"/>
@@ -1795,7 +2076,7 @@
       <c r="H47" s="24"/>
       <c r="I47" s="33"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="30"/>
       <c r="C48" s="30"/>
@@ -1806,7 +2087,7 @@
       <c r="H48" s="24"/>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="30"/>
       <c r="B49" s="30"/>
       <c r="C49" s="30"/>
@@ -1817,7 +2098,7 @@
       <c r="H49" s="24"/>
       <c r="I49" s="33"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="30"/>
       <c r="C50" s="30"/>
@@ -1828,7 +2109,7 @@
       <c r="H50" s="24"/>
       <c r="I50" s="33"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="30"/>
       <c r="C51" s="30"/>
@@ -1839,7 +2120,7 @@
       <c r="H51" s="24"/>
       <c r="I51" s="33"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="30"/>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -1850,7 +2131,7 @@
       <c r="H52" s="24"/>
       <c r="I52" s="33"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="30"/>
       <c r="B53" s="30"/>
       <c r="C53" s="30"/>
@@ -1863,44 +2144,39 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>#ref!</formula>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1 G15:G1053" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G15:G1053" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$5:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1053" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1053" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$14:$K$14</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G14" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updating SIQ sheet - CYRS review (close all points except one) - HSI review (Close point 2,3,5 and 6 also open 8 and 9 ) Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moamen\Desktop\SWE\Input documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A013E-0F78-4700-B192-BF704E343A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
   <definedNames>
     <definedName name="_Toc30697436" localSheetId="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -269,18 +263,24 @@
   <si>
     <t xml:space="preserve">Is for the reviewer he check the fix of the open point and check if the fix is ok or still open </t>
   </si>
+  <si>
+    <t>Mali 7/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>Mali 7/2/2020: Point is reviewed and closed, Features section is removed although there is no comment about this in the history</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-409]General"/>
     <numFmt numFmtId="167" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -524,41 +524,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -624,14 +591,212 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Accent3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Excel Built-in Accent3" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3 2" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFBE5D6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF535353"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF808080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFBE5D6"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF1F4E79"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDAE3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF385724"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF535353"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBDBDB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF808080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -816,7 +981,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -868,7 +1033,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1062,210 +1227,234 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:M18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:13">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="31"/>
+      <c r="G12" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="14">
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="3">
         <v>0.1</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="3"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="3"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="3"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="3"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="4"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1275,30 +1464,6 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1306,14 +1471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -1322,417 +1487,440 @@
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="106.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="9" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
     <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" ht="34.15" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:11" ht="30">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="24"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="H2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="24"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="H3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="24"/>
+      <c r="H4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>59</v>
+      </c>
       <c r="K4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:11" ht="30">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="24"/>
+      <c r="H5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>59</v>
+      </c>
       <c r="K5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="24"/>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" ht="45">
+      <c r="A7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="24"/>
-    </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="H7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45">
+      <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="H8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30">
+      <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="H9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120">
+      <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="24"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="H10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90">
+      <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="H11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="61.5">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="H12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23" t="s">
+      <c r="H13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="22"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
       <c r="K14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="22"/>
+    <row r="15" spans="1:11">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
       <c r="K17" t="s">
         <v>55</v>
       </c>
@@ -1740,16 +1928,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="22"/>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
       <c r="K18" t="s">
         <v>57</v>
       </c>
@@ -1757,421 +1945,429 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="33"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="33"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="33"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="33"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="33"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="33"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="33"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="33"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="33"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="33"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="33"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="33"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="33"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="33"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="33"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="33"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="33"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="33"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="33"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="33"/>
+    <row r="19" spans="1:12">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="22"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="22"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="22"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="22"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="22"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="22"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="22"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="22"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="22"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="22"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="22"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="22"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="22"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="22"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="22"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="22"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Resolved"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G15:G1053" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G15:G1053">
       <formula1>$K$5:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1053" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1053">
       <formula1>$K$14:$K$14</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14">
       <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Release CYRS Update review sheet for HSI Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">Status of document must be changed from Draft to Proposed and then Releases after accomplishing cross review on it. </t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>All pages</t>
@@ -591,47 +588,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -640,19 +637,7 @@
     <cellStyle name="Normal 3 2" xfId="1"/>
     <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <condense val="0"/>
@@ -674,126 +659,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF385724"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF535353"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF808080"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFBE5D6"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF1F4E79"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDAE3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF385724"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF535353"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDBDBDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF808080"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1227,7 +1092,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1247,214 +1112,190 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="35" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="32"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="3">
         <v>0.1</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="37"/>
+      <c r="E13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29" t="s">
+      <c r="F13" s="37"/>
+      <c r="G13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="3"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="3"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="3"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="3"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="4"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
@@ -1464,6 +1305,30 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1474,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1487,7 +1352,7 @@
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="106.28515625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="28" customWidth="1"/>
     <col min="9" max="9" width="23.85546875" customWidth="1"/>
     <col min="12" max="12" width="174.28515625" customWidth="1"/>
   </cols>
@@ -1541,13 +1406,13 @@
         <v>29</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30">
@@ -1564,19 +1429,19 @@
         <v>27</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30">
@@ -1593,22 +1458,22 @@
         <v>27</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="H4" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30">
@@ -1625,22 +1490,22 @@
         <v>27</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1657,16 +1522,16 @@
         <v>27</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="G6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="I6" s="13"/>
     </row>
@@ -1684,19 +1549,19 @@
         <v>27</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45">
@@ -1713,19 +1578,19 @@
         <v>27</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>44</v>
-      </c>
       <c r="G8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30">
@@ -1742,19 +1607,19 @@
         <v>27</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>46</v>
-      </c>
       <c r="G9" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="120">
@@ -1771,19 +1636,19 @@
         <v>27</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>48</v>
-      </c>
       <c r="G10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I10" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="90">
@@ -1800,19 +1665,19 @@
         <v>27</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="38" t="s">
-        <v>50</v>
-      </c>
       <c r="G11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="61.5">
@@ -1829,19 +1694,19 @@
         <v>27</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60">
@@ -1858,19 +1723,19 @@
         <v>27</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="37" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30">
@@ -1880,13 +1745,13 @@
       <c r="D14" s="9"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1922,10 +1787,10 @@
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" t="s">
         <v>55</v>
-      </c>
-      <c r="L17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1939,10 +1804,10 @@
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="K18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" t="s">
         <v>57</v>
-      </c>
-      <c r="L18" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2332,29 +2197,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H13">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Resolved"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>